<commit_message>
Peer Review has been done
</commit_message>
<xml_diff>
--- a/Car_TestCases/Car_AdminTCs.xlsx
+++ b/Car_TestCases/Car_AdminTCs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="81">
   <si>
     <t>Test case ID</t>
   </si>
@@ -324,6 +324,9 @@
   </si>
   <si>
     <t xml:space="preserve">The admin can't add user and error message displayed as "please fill out this field". </t>
+  </si>
+  <si>
+    <t>Mina</t>
   </si>
 </sst>
 </file>
@@ -773,22 +776,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="H13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="16.42578125" style="6"/>
-    <col min="4" max="4" width="34.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" style="6" customWidth="1"/>
+    <col min="1" max="3" width="16.44140625" style="6"/>
+    <col min="4" max="4" width="34.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="36.109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" style="6" customWidth="1"/>
     <col min="7" max="7" width="49" style="6" customWidth="1"/>
-    <col min="8" max="8" width="36.140625" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="16.42578125" style="6"/>
+    <col min="8" max="8" width="36.109375" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="16.44140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="5" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" s="5" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -844,7 +847,7 @@
       <c r="AA1" s="3"/>
       <c r="AB1" s="4"/>
     </row>
-    <row r="2" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
@@ -872,8 +875,11 @@
       <c r="K2" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="190.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -901,8 +907,11 @@
       <c r="K3" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
@@ -933,8 +942,11 @@
       <c r="K4" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -962,8 +974,11 @@
       <c r="K5" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="169.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
@@ -991,8 +1006,11 @@
       <c r="K6" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="169.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
@@ -1020,8 +1038,11 @@
       <c r="K7" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="169.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
@@ -1049,8 +1070,11 @@
       <c r="K8" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M8" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
@@ -1078,8 +1102,11 @@
       <c r="K9" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>53</v>
       </c>
@@ -1110,8 +1137,11 @@
       <c r="K10" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M10" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="116.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>54</v>
       </c>
@@ -1142,8 +1172,11 @@
       <c r="K11" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="109.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>55</v>
       </c>
@@ -1174,8 +1207,11 @@
       <c r="K12" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>68</v>
       </c>
@@ -1206,8 +1242,11 @@
       <c r="K13" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>69</v>
       </c>
@@ -1234,6 +1273,9 @@
       </c>
       <c r="K14" s="6" t="s">
         <v>25</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated & reviewed AdminTCs
</commit_message>
<xml_diff>
--- a/Car_TestCases/Car_AdminTCs.xlsx
+++ b/Car_TestCases/Car_AdminTCs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
   <si>
     <t>Test case ID</t>
   </si>
@@ -324,9 +324,6 @@
   </si>
   <si>
     <t xml:space="preserve">The admin can't add user and error message displayed as "please fill out this field". </t>
-  </si>
-  <si>
-    <t>Mina</t>
   </si>
 </sst>
 </file>
@@ -776,22 +773,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="16.44140625" style="6"/>
-    <col min="4" max="4" width="34.6640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="36.109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" style="6" customWidth="1"/>
+    <col min="1" max="3" width="16.42578125" style="6"/>
+    <col min="4" max="4" width="34.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" style="6" customWidth="1"/>
     <col min="7" max="7" width="49" style="6" customWidth="1"/>
-    <col min="8" max="8" width="36.109375" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="16.44140625" style="6"/>
+    <col min="8" max="8" width="36.140625" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="16.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="5" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" s="5" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -847,7 +844,7 @@
       <c r="AA1" s="3"/>
       <c r="AB1" s="4"/>
     </row>
-    <row r="2" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
@@ -875,11 +872,8 @@
       <c r="K2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" ht="190.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:28" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -907,11 +901,8 @@
       <c r="K3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
@@ -942,11 +933,8 @@
       <c r="K4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -974,11 +962,8 @@
       <c r="K5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" ht="169.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:28" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
@@ -1006,11 +991,8 @@
       <c r="K6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M6" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" ht="169.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:28" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
@@ -1038,11 +1020,8 @@
       <c r="K7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" ht="169.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:28" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
@@ -1070,14 +1049,14 @@
       <c r="K8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M8" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="B9" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="C9" s="6" t="s">
         <v>24</v>
       </c>
@@ -1102,11 +1081,8 @@
       <c r="K9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M9" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>53</v>
       </c>
@@ -1137,11 +1113,8 @@
       <c r="K10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" ht="116.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:28" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>54</v>
       </c>
@@ -1172,11 +1145,8 @@
       <c r="K11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M11" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" ht="109.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:28" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>55</v>
       </c>
@@ -1207,11 +1177,8 @@
       <c r="K12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M12" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:28" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>68</v>
       </c>
@@ -1242,11 +1209,8 @@
       <c r="K13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M13" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:28" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>69</v>
       </c>
@@ -1273,9 +1237,6 @@
       </c>
       <c r="K14" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>